<commit_message>
Allow duplicate searching and choosing ID
</commit_message>
<xml_diff>
--- a/app/config/tables/registration/forms/registration/registration.xlsx
+++ b/app/config/tables/registration/forms/registration/registration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ray\Research\app-designer\app\config\tables\registration\forms\registration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A3855E-4EE1-494D-B491-F4759D256845}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DA2777-F6C4-44C4-BC65-C021806312CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{18E54974-4CA3-4ADB-B752-9A6313405798}"/>
+    <workbookView xWindow="970" yWindow="530" windowWidth="14400" windowHeight="7810" xr2:uid="{18E54974-4CA3-4ADB-B752-9A6313405798}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -155,40 +155,40 @@
     <t>client_id</t>
   </si>
   <si>
-    <t>The UUID of the client is:</t>
-  </si>
-  <si>
     <t>Please write down this ID and don't lose it</t>
   </si>
   <si>
-    <t>What is your client's first name?</t>
-  </si>
-  <si>
-    <t>What is your client's middle name?</t>
-  </si>
-  <si>
-    <t>What is your client's surname?</t>
-  </si>
-  <si>
-    <t>What is your client's assigned birth sex?</t>
-  </si>
-  <si>
-    <t>When was your client born?</t>
-  </si>
-  <si>
-    <t>Where does your client live?</t>
-  </si>
-  <si>
-    <t>What country did your client live in?</t>
-  </si>
-  <si>
-    <t>What is your client's telephone number?</t>
-  </si>
-  <si>
-    <t>What is your client's father's name?</t>
-  </si>
-  <si>
-    <t>What is your client's mother's name?</t>
+    <t>Please choose an ID for the patient:</t>
+  </si>
+  <si>
+    <t>What is your patient's first name?</t>
+  </si>
+  <si>
+    <t>What is your patient's middle name?</t>
+  </si>
+  <si>
+    <t>What is your patient's surname?</t>
+  </si>
+  <si>
+    <t>What is your patient's assigned birth sex?</t>
+  </si>
+  <si>
+    <t>When was your patient born?</t>
+  </si>
+  <si>
+    <t>Where does your patient live?</t>
+  </si>
+  <si>
+    <t>What country does your patient live in?</t>
+  </si>
+  <si>
+    <t>What is your patient's telephone number?</t>
+  </si>
+  <si>
+    <t>What is your patient's father's name?</t>
+  </si>
+  <si>
+    <t>What is your patient's mother's name?</t>
   </si>
 </sst>
 </file>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2897AAC8-9D28-46CB-A7FE-82CEFB9B5D98}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -596,10 +596,10 @@
         <v>39</v>
       </c>
       <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" t="s">
         <v>40</v>
-      </c>
-      <c r="I2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>